<commit_message>
Update ASV and synthetic files
</commit_message>
<xml_diff>
--- a/metadata/Singapore_metadata.xlsx
+++ b/metadata/Singapore_metadata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\daniel.vaulot@gmail.com\Metabarcoding\Singapore\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D935E57C-05C4-49D0-BA13-2E7876D95377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0E0E42-BDF5-48F7-96E5-2DE8D95DFC15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11220" xr2:uid="{4D804F22-DFAA-47B5-8477-9C86D93AA77B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11220" activeTab="1" xr2:uid="{4D804F22-DFAA-47B5-8477-9C86D93AA77B}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="stations" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">metadata!$A$1:$S$86</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="294">
   <si>
     <t>sample_id</t>
   </si>
@@ -911,6 +912,12 @@
   </si>
   <si>
     <t>sequence_quality</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
@@ -920,7 +927,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -928,8 +935,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,12 +952,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,8 +973,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1284,9 +1293,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DD33BE-8376-466B-AC6A-1AAF9615F942}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3438,11 +3447,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2671CF9F-3B5F-4DBB-A701-D335868C899A}">
   <dimension ref="A1:S86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" ySplit="1" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3571,7 +3580,7 @@
       <c r="A3" s="2">
         <v>37</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>42772</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3597,7 +3606,7 @@
       <c r="A4" s="2">
         <v>37</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>42772</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -4870,7 +4879,7 @@
       <c r="A30" s="2">
         <v>247</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>42984</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -5151,7 +5160,7 @@
         <v>9</v>
       </c>
       <c r="G35" t="s">
-        <v>282</v>
+        <v>83</v>
       </c>
       <c r="H35">
         <v>45.4</v>
@@ -5188,7 +5197,7 @@
       <c r="B36" s="3">
         <v>43034</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>272</v>
       </c>
       <c r="D36" t="s">
@@ -5300,7 +5309,7 @@
       <c r="A38" s="2">
         <v>299</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>43034</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -8108,4 +8117,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF46FDCF-F5A5-4982-9389-AAE586DF9FA0}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2">
+        <v>1.2383194</v>
+      </c>
+      <c r="D2">
+        <v>103.85355149999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>1.2972229</v>
+      </c>
+      <c r="D3">
+        <v>103.920675</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>1.3885730999999999</v>
+      </c>
+      <c r="D4">
+        <v>103.9514805</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5">
+        <v>1.4716237000000001</v>
+      </c>
+      <c r="D5">
+        <v>103.80508330000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1.3446619</v>
+      </c>
+      <c r="D6" s="5">
+        <v>103.6340957</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates after meeting with Fede
</commit_message>
<xml_diff>
--- a/metadata/Singapore_metadata.xlsx
+++ b/metadata/Singapore_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\daniel.vaulot@gmail.com\Metabarcoding\Singapore\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0E0E42-BDF5-48F7-96E5-2DE8D95DFC15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE424EB8-1806-4CC8-BD2E-C89A86F5A144}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11220" activeTab="1" xr2:uid="{4D804F22-DFAA-47B5-8477-9C86D93AA77B}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">metadata!$A$1:$S$86</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">samples!$A$1:$K$89</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="294">
   <si>
     <t>sample_id</t>
   </si>
@@ -3448,10 +3449,10 @@
   <dimension ref="A1:S86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomRight" activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6435,7 +6436,7 @@
       <c r="H58">
         <v>0</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J58">
@@ -6494,8 +6495,8 @@
       <c r="H59">
         <v>0</v>
       </c>
-      <c r="I59" t="s">
-        <v>184</v>
+      <c r="I59" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="J59">
         <v>1.98</v>
@@ -6553,8 +6554,8 @@
       <c r="H60">
         <v>0.5</v>
       </c>
-      <c r="I60" t="s">
-        <v>184</v>
+      <c r="I60" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="J60">
         <v>2.2000000000000002</v>
@@ -6612,8 +6613,8 @@
       <c r="H61">
         <v>3</v>
       </c>
-      <c r="I61" t="s">
-        <v>184</v>
+      <c r="I61" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="J61">
         <v>57.46</v>
@@ -6671,8 +6672,8 @@
       <c r="H62">
         <v>0</v>
       </c>
-      <c r="I62" t="s">
-        <v>184</v>
+      <c r="I62" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="K62">
         <v>28.2</v>
@@ -8111,7 +8112,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:S86" xr:uid="{51958C7C-4D2C-458C-8A1B-8FE35E4A2E01}"/>
-  <sortState ref="A2:S167">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S167">
     <sortCondition ref="A2:A167"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>